<commit_message>
* Finished adding built-in operators, except '__and__' and '__or__' * 'if' statement was added (work in progress) * Recursive function type calculation was added (work in progress)
</commit_message>
<xml_diff>
--- a/Docs/BuiltIns.xlsx
+++ b/Docs/BuiltIns.xlsx
@@ -134,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,11 +159,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="darkDown">
-        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,7 +187,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -494,7 +489,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -656,11 +651,11 @@
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -678,11 +673,11 @@
       <c r="P7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="R7" s="6"/>
-      <c r="S7" t="s">
+      <c r="S7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="V7" s="5">
@@ -749,11 +744,11 @@
       <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -771,11 +766,11 @@
       <c r="P9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="R9" s="6"/>
-      <c r="S9" t="s">
+      <c r="S9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -833,11 +828,11 @@
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="6"/>
-      <c r="I12" t="s">
+      <c r="I12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -901,11 +896,11 @@
       <c r="F14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" t="s">
+      <c r="I14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -975,11 +970,11 @@
       <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" t="s">
+      <c r="I17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1043,11 +1038,11 @@
       <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="I19" t="s">
+      <c r="I19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -1114,11 +1109,11 @@
       <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" t="s">
+      <c r="I22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L22" s="4" t="s">

</xml_diff>